<commit_message>
trying to get npm working again
</commit_message>
<xml_diff>
--- a/grade-estimator/test/Expected values.xlsx
+++ b/grade-estimator/test/Expected values.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Dropbox/gradeestimator/grade-estimator/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B909CD92-1E6C-5547-BB23-72B06E1CF21F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1401D595-A840-D546-8C3F-4EAC4907DF1E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="17000" windowHeight="17040" xr2:uid="{091BDCF0-A9AC-074C-9DDD-BF960AA8A237}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="alt" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>P/A</t>
   </si>
@@ -64,6 +71,15 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>each oa</t>
+  </si>
+  <si>
+    <t>each journal</t>
   </si>
 </sst>
 </file>
@@ -443,7 +459,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,11 +538,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G3" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1">
         <f>G3*$B$3</f>
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -551,11 +567,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G4" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
         <f>G4*$B$4</f>
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -609,11 +625,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G6" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f>G6*$B$6</f>
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -753,7 +769,390 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1">
         <f>SUM(H2:H10)</f>
-        <v>55</v>
+        <v>48.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE5FA5B-5B86-A94E-A034-CD85EA1430FF}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <f>100*B2</f>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>95</v>
+      </c>
+      <c r="E2" s="1">
+        <f>(D2+5)*B2</f>
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2">
+        <f>(F2+5)*$B$2</f>
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>55</v>
+      </c>
+      <c r="I2" s="1">
+        <f>H2*$B$2</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.04</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C10" si="0">100*B3</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E10" si="1">(D3+5)*B3</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>55</v>
+      </c>
+      <c r="G3" s="2">
+        <f>F3*$B$3</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <v>55</v>
+      </c>
+      <c r="I3" s="1">
+        <f>H3*$B$3</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.04</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>95</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2">
+        <f>F4*$B$4</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H4" s="1">
+        <v>55</v>
+      </c>
+      <c r="I4" s="1">
+        <f>H4*$B$4</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.04</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2">
+        <f>F5*$B$5</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <v>55</v>
+      </c>
+      <c r="I5" s="1">
+        <f>H5*$B$5</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.04</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>55</v>
+      </c>
+      <c r="G6" s="2">
+        <f>F6*$B$6</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H6" s="1">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1">
+        <f>H6*$B$6</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0.04</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>95</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2">
+        <f>F7*$B$7</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H7" s="1">
+        <v>55</v>
+      </c>
+      <c r="I7" s="1">
+        <f>H7*$B$7</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.05</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>95</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>55</v>
+      </c>
+      <c r="G8" s="2">
+        <f>F8*$B$8</f>
+        <v>2.75</v>
+      </c>
+      <c r="H8" s="1">
+        <v>55</v>
+      </c>
+      <c r="I8" s="1">
+        <f>H8*$B$8</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.35</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D9" s="1">
+        <v>95</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="F9" s="2">
+        <v>55</v>
+      </c>
+      <c r="G9" s="2">
+        <f>F9*$B$9</f>
+        <v>19.25</v>
+      </c>
+      <c r="H9" s="1">
+        <v>55</v>
+      </c>
+      <c r="I9" s="1">
+        <f>H9*$B$9</f>
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.3</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>95</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="2">
+        <v>55</v>
+      </c>
+      <c r="G10" s="2">
+        <f>F10*$B$10</f>
+        <v>16.5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>55</v>
+      </c>
+      <c r="I10" s="1">
+        <f>H10*$B$10</f>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2:B10)</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>SUM(C2:C10)</f>
+        <v>100</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <f>SUM(E2:E10)</f>
+        <v>100</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <f>SUM(G2:G10)</f>
+        <v>55.5</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <f>SUM(I2:I10)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f>5/15</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>